<commit_message>
Updated user name and password to the actual contents
</commit_message>
<xml_diff>
--- a/Config/Config.xlsx
+++ b/Config/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tharusha Jayadeera\Documents\UiPath\Extract_Address_From_Gmail\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{637FA730-B042-4780-979C-E720163EFA83}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D57FF987-D9A2-493F-B908-0BE7BD332D23}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,12 +34,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>tharushauipath1@gmail.com</t>
-  </si>
-  <si>
-    <t>tharusha1996</t>
-  </si>
-  <si>
     <t>ClientID</t>
   </si>
   <si>
@@ -50,6 +44,12 @@
   </si>
   <si>
     <t>FWbhjEx57cVr4kTwl0ntn286</t>
+  </si>
+  <si>
+    <t>yourrealtyautomation1@gmail.com</t>
+  </si>
+  <si>
+    <t>6754auto</t>
   </si>
 </sst>
 </file>
@@ -418,9 +418,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
@@ -492,7 +490,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
@@ -500,24 +498,24 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="1:25" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:25" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>